<commit_message>
Merged changes up to tag v241018: implemented evoked beamformer src reconstruction; added new steps 'plot_waveforms', 'plot_epochs'; hardcoded Nancy's wrong sIDs as valid sIDs
</commit_message>
<xml_diff>
--- a/description/processing.xlsx
+++ b/description/processing.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="116">
   <si>
     <t xml:space="preserve">Subject ID</t>
   </si>
@@ -41,7 +41,10 @@
     <t xml:space="preserve">bem</t>
   </si>
   <si>
-    <t xml:space="preserve">src</t>
+    <t xml:space="preserve">Src act [0,4]s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Src act [1,3.5]s</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -71,6 +74,12 @@
     <t xml:space="preserve">4ESU5W</t>
   </si>
   <si>
+    <t xml:space="preserve">52C4TG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no bem</t>
+  </si>
+  <si>
     <t xml:space="preserve">54RWW6</t>
   </si>
   <si>
@@ -137,7 +146,7 @@
     <t xml:space="preserve">DEDNDJ</t>
   </si>
   <si>
-    <t xml:space="preserve">fail</t>
+    <t xml:space="preserve">rest, nat DONE</t>
   </si>
   <si>
     <t xml:space="preserve">Can’t epoch – no event 41</t>
@@ -158,19 +167,22 @@
     <t xml:space="preserve">ET2PJN</t>
   </si>
   <si>
-    <t xml:space="preserve">EXT6ADJ3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTMCJQKQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTRTPD9A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTTVFMU4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTU2M7EY</t>
+    <t xml:space="preserve">ext6ADJ3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extFQABY7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extMCJQKQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extRTPD9A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extTVFMU4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extU2M7EY</t>
   </si>
   <si>
     <t xml:space="preserve">F2ESKX</t>
@@ -200,7 +212,7 @@
     <t xml:space="preserve">HB57WT</t>
   </si>
   <si>
-    <t xml:space="preserve">!!! Corresponds to YYQQF9 on MRI side !!!</t>
+    <t xml:space="preserve">??? Nancy: Corresponds to YYQQF9 on MRI side ??? – not really</t>
   </si>
   <si>
     <t xml:space="preserve">HCUZQ4</t>
@@ -224,12 +236,12 @@
     <t xml:space="preserve">JYBZXP</t>
   </si>
   <si>
-    <t xml:space="preserve">not ready</t>
-  </si>
-  <si>
     <t xml:space="preserve">K83Z5S</t>
   </si>
   <si>
+    <t xml:space="preserve">KAGAJY</t>
+  </si>
+  <si>
     <t xml:space="preserve">KETDQV</t>
   </si>
   <si>
@@ -263,6 +275,9 @@
     <t xml:space="preserve">NTDU8N</t>
   </si>
   <si>
+    <t xml:space="preserve">NTQYDM</t>
+  </si>
+  <si>
     <t xml:space="preserve">PAWEZ5</t>
   </si>
   <si>
@@ -305,6 +320,9 @@
     <t xml:space="preserve">US5GA6</t>
   </si>
   <si>
+    <t xml:space="preserve">UTCZ7P</t>
+  </si>
+  <si>
     <t xml:space="preserve">V9HDQM</t>
   </si>
   <si>
@@ -338,6 +356,12 @@
     <t xml:space="preserve">YAY7MU</t>
   </si>
   <si>
+    <t xml:space="preserve">YRGNZY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has retainers; all channels bad quality</t>
+  </si>
+  <si>
     <t xml:space="preserve">YYQQF8</t>
   </si>
   <si>
@@ -345,12 +369,6 @@
   </si>
   <si>
     <t xml:space="preserve">Total done:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ext6ADJ3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extMCJQKQ</t>
   </si>
 </sst>
 </file>
@@ -658,17 +676,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J94"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G79" activeCellId="0" sqref="G79"/>
+      <selection pane="bottomLeft" activeCell="H101" activeCellId="0" sqref="H101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="29.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="29.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,19 +710,22 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>1</v>
@@ -719,11 +742,14 @@
       <c r="G2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="H2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>1</v>
@@ -740,11 +766,14 @@
       <c r="G3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J3" s="3"/>
+      <c r="H3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>1</v>
@@ -761,11 +790,14 @@
       <c r="G4" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="H4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>1</v>
@@ -774,12 +806,21 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>1</v>
@@ -796,11 +837,14 @@
       <c r="G6" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J6" s="3"/>
+      <c r="H6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>1</v>
@@ -817,11 +861,14 @@
       <c r="G7" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J7" s="3"/>
+      <c r="H7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>1</v>
@@ -838,25 +885,28 @@
       <c r="G8" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J8" s="3"/>
+      <c r="H8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3" t="n">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>1</v>
@@ -865,12 +915,21 @@
         <v>1</v>
       </c>
       <c r="E10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>1</v>
@@ -879,12 +938,21 @@
         <v>1</v>
       </c>
       <c r="E11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>1</v>
@@ -893,12 +961,21 @@
         <v>1</v>
       </c>
       <c r="E12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>1</v>
@@ -912,7 +989,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>1</v>
@@ -921,12 +998,21 @@
         <v>1</v>
       </c>
       <c r="E14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>1</v>
@@ -935,12 +1021,21 @@
         <v>1</v>
       </c>
       <c r="E15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>1</v>
@@ -951,17 +1046,19 @@
       <c r="E16" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16" s="3"/>
+      <c r="F16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>1</v>
@@ -972,11 +1069,20 @@
       <c r="E17" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J17" s="3"/>
+      <c r="F17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>1</v>
@@ -987,11 +1093,20 @@
       <c r="E18" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J18" s="3"/>
+      <c r="F18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>1</v>
@@ -1002,17 +1117,20 @@
       <c r="E19" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F19" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J19" s="3"/>
+      <c r="F19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>1</v>
@@ -1029,11 +1147,14 @@
       <c r="G20" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J20" s="3"/>
+      <c r="H20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>1</v>
@@ -1050,11 +1171,14 @@
       <c r="G21" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J21" s="3"/>
+      <c r="H21" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>1</v>
@@ -1071,11 +1195,14 @@
       <c r="G22" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J22" s="3"/>
+      <c r="H22" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>1</v>
@@ -1092,11 +1219,14 @@
       <c r="G23" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J23" s="3"/>
+      <c r="H23" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>1</v>
@@ -1113,10 +1243,14 @@
       <c r="G24" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="H24" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>1</v>
@@ -1125,12 +1259,21 @@
         <v>1</v>
       </c>
       <c r="E25" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>1</v>
@@ -1141,19 +1284,19 @@
       <c r="E26" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F26" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G26" s="3" t="n">
+      <c r="F26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="4" t="n">
-        <v>45225</v>
+        <v>36</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>1</v>
@@ -1162,12 +1305,24 @@
         <v>1</v>
       </c>
       <c r="E27" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="B28" s="4" t="n">
+        <v>45225</v>
       </c>
       <c r="C28" s="3" t="n">
         <v>1</v>
@@ -1178,17 +1333,19 @@
       <c r="E28" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F28" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J28" s="3"/>
+      <c r="F28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>1</v>
@@ -1199,11 +1356,20 @@
       <c r="E29" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J29" s="3"/>
+      <c r="F29" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C30" s="3" t="n">
         <v>1</v>
@@ -1214,16 +1380,16 @@
       <c r="E30" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F30" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="3"/>
+      <c r="F30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
@@ -1238,11 +1404,23 @@
       <c r="E31" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J31" s="3"/>
+      <c r="F31" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C32" s="3" t="n">
         <v>1</v>
@@ -1253,11 +1431,20 @@
       <c r="E32" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J32" s="3"/>
+      <c r="F32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C33" s="3" t="n">
         <v>1</v>
@@ -1268,10 +1455,20 @@
       <c r="E33" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="F33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C34" s="3" t="n">
         <v>1</v>
@@ -1282,16 +1479,19 @@
       <c r="E34" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F34" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G34" s="3" t="n">
+      <c r="F34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C35" s="3" t="n">
         <v>1</v>
@@ -1302,44 +1502,134 @@
       <c r="E35" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="F35" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3" t="n">
+      <c r="A36" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H40" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
-        <v>50</v>
+      <c r="A41" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="C41" s="3" t="n">
         <v>1</v>
@@ -1350,26 +1640,42 @@
       <c r="E41" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F41" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G41" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J41" s="3"/>
+      <c r="F41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F42" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J42" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="C42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C43" s="3" t="n">
         <v>1</v>
@@ -1386,11 +1692,14 @@
       <c r="G43" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J43" s="3"/>
+      <c r="H43" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
-        <v>53</v>
+      <c r="A44" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C44" s="3" t="n">
         <v>1</v>
@@ -1401,17 +1710,20 @@
       <c r="E44" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F44" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G44" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J44" s="3"/>
+      <c r="F44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C45" s="3" t="n">
         <v>1</v>
@@ -1428,11 +1740,14 @@
       <c r="G45" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J45" s="3"/>
+      <c r="H45" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C46" s="3" t="n">
         <v>1</v>
@@ -1449,11 +1764,14 @@
       <c r="G46" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J46" s="3"/>
+      <c r="H46" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C47" s="3" t="n">
         <v>1</v>
@@ -1464,11 +1782,20 @@
       <c r="E47" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J47" s="3"/>
+      <c r="F47" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C48" s="3" t="n">
         <v>1</v>
@@ -1485,11 +1812,14 @@
       <c r="G48" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J48" s="3"/>
+      <c r="H48" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C49" s="3" t="n">
         <v>1</v>
@@ -1500,14 +1830,20 @@
       <c r="E49" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H49" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J49" s="3"/>
+      <c r="F49" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C50" s="3" t="n">
         <v>1</v>
@@ -1518,11 +1854,20 @@
       <c r="E50" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J50" s="3"/>
+      <c r="F50" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C51" s="3" t="n">
         <v>1</v>
@@ -1533,16 +1878,23 @@
       <c r="E51" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F51" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G51" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="F51" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C52" s="3" t="n">
         <v>1</v>
@@ -1553,10 +1905,20 @@
       <c r="E52" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="F52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C53" s="3" t="n">
         <v>1</v>
@@ -1565,12 +1927,21 @@
         <v>1</v>
       </c>
       <c r="E53" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G53" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C54" s="3" t="n">
         <v>1</v>
@@ -1581,16 +1952,19 @@
       <c r="E54" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F54" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G54" s="3" t="n">
+      <c r="F54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H54" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C55" s="3" t="n">
         <v>1</v>
@@ -1601,16 +1975,19 @@
       <c r="E55" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F55" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G55" s="3" t="n">
+      <c r="F55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C56" s="3" t="n">
         <v>1</v>
@@ -1621,14 +1998,19 @@
       <c r="E56" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F56" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G56" s="3"/>
+      <c r="F56" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G56" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H56" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C57" s="3" t="n">
         <v>1</v>
@@ -1645,11 +2027,13 @@
       <c r="G57" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J57" s="3"/>
+      <c r="H57" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C58" s="3" t="n">
         <v>1</v>
@@ -1666,11 +2050,13 @@
       <c r="G58" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J58" s="3"/>
+      <c r="H58" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C59" s="3" t="n">
         <v>1</v>
@@ -1681,11 +2067,20 @@
       <c r="E59" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J59" s="3"/>
+      <c r="F59" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G59" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C60" s="3" t="n">
         <v>1</v>
@@ -1696,11 +2091,20 @@
       <c r="E60" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J60" s="3"/>
+      <c r="F60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C61" s="3" t="n">
         <v>1</v>
@@ -1717,11 +2121,14 @@
       <c r="G61" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J61" s="3"/>
+      <c r="H61" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C62" s="3" t="n">
         <v>1</v>
@@ -1732,11 +2139,11 @@
       <c r="E62" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C63" s="3" t="n">
         <v>1</v>
@@ -1747,11 +2154,20 @@
       <c r="E63" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J63" s="3"/>
+      <c r="F63" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C64" s="3" t="n">
         <v>1</v>
@@ -1768,10 +2184,10 @@
       <c r="G64" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H64" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J64" s="3"/>
+      <c r="H64" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
@@ -1786,13 +2202,7 @@
       <c r="E65" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F65" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G65" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
@@ -1807,7 +2217,16 @@
       <c r="E66" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J66" s="3"/>
+      <c r="F66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
@@ -1828,11 +2247,17 @@
       <c r="G67" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J67" s="3"/>
+      <c r="H67" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C68" s="3" t="n">
         <v>1</v>
@@ -1849,11 +2274,14 @@
       <c r="G68" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J68" s="3"/>
+      <c r="H68" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C69" s="3" t="n">
         <v>1</v>
@@ -1864,17 +2292,20 @@
       <c r="E69" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F69" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G69" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J69" s="3"/>
+      <c r="F69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C70" s="3" t="n">
         <v>1</v>
@@ -1891,32 +2322,28 @@
       <c r="G70" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J70" s="3"/>
+      <c r="H70" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C71" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D71" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E71" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F71" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G71" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J71" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="K71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C72" s="3" t="n">
         <v>1</v>
@@ -1933,11 +2360,14 @@
       <c r="G72" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J72" s="3"/>
+      <c r="H72" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C73" s="3" t="n">
         <v>1</v>
@@ -1948,20 +2378,44 @@
       <c r="E73" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J73" s="3"/>
+      <c r="F73" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G73" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H73" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="s">
-        <v>86</v>
+      <c r="A74" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C74" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D74" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E74" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="F74" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J74" s="3"/>
+      <c r="G74" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H74" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C75" s="3" t="n">
         <v>1</v>
@@ -1978,11 +2432,14 @@
       <c r="G75" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J75" s="3"/>
+      <c r="H75" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C76" s="3" t="n">
         <v>1</v>
@@ -1999,11 +2456,14 @@
       <c r="G76" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J76" s="3"/>
+      <c r="H76" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C77" s="3" t="n">
         <v>1</v>
@@ -2014,15 +2474,20 @@
       <c r="E77" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F77" s="3"/>
-      <c r="G77" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J77" s="3"/>
+      <c r="F77" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G77" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H77" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3" t="s">
-        <v>90</v>
+      <c r="A78" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="C78" s="3" t="n">
         <v>1</v>
@@ -2036,14 +2501,17 @@
       <c r="F78" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G78" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J78" s="3"/>
+      <c r="G78" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H78" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C79" s="3" t="n">
         <v>1</v>
@@ -2054,10 +2522,16 @@
       <c r="E79" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H79" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="J79" s="3"/>
+      <c r="F79" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G79" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H79" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K79" s="3"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
@@ -2078,10 +2552,10 @@
       <c r="G80" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J80" s="3" t="str">
-        <f aca="false">IF(AND(E80="done", F80="done"), A80, "")</f>
-        <v/>
-      </c>
+      <c r="H80" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
@@ -2102,10 +2576,10 @@
       <c r="G81" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J81" s="3" t="str">
-        <f aca="false">IF(AND(E81="done", F81="done"), A81, "")</f>
-        <v/>
-      </c>
+      <c r="H81" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
@@ -2120,16 +2594,16 @@
       <c r="E82" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F82" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G82" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" s="3" t="str">
-        <f aca="false">IF(AND(E82="done", F82="done"), A82, "")</f>
-        <v/>
-      </c>
+      <c r="F82" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G82" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H82" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
@@ -2144,20 +2618,23 @@
       <c r="E83" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F83" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G83" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J83" s="3" t="str">
-        <f aca="false">IF(AND(E83="done", F83="done"), A83, "")</f>
-        <v/>
-      </c>
+      <c r="F83" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G83" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H83" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K83" s="3"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C84" s="3" t="n">
         <v>1</v>
@@ -2168,14 +2645,23 @@
       <c r="E84" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J84" s="3" t="str">
+      <c r="F84" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G84" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H84" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K84" s="3" t="str">
         <f aca="false">IF(AND(E84="done", F84="done"), A84, "")</f>
         <v/>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C85" s="3" t="n">
         <v>1</v>
@@ -2186,20 +2672,20 @@
       <c r="E85" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F85" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G85" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J85" s="3" t="str">
-        <f aca="false">IF(AND(E85="done", F85="done"), A85, "")</f>
-        <v/>
-      </c>
+      <c r="F85" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G85" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H85" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K85" s="3"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C86" s="3" t="n">
         <v>1</v>
@@ -2216,14 +2702,17 @@
       <c r="G86" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J86" s="3" t="str">
+      <c r="H86" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K86" s="3" t="str">
         <f aca="false">IF(AND(E86="done", F86="done"), A86, "")</f>
         <v/>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C87" s="3" t="n">
         <v>1</v>
@@ -2234,14 +2723,23 @@
       <c r="E87" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J87" s="3" t="str">
+      <c r="F87" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G87" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H87" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K87" s="3" t="str">
         <f aca="false">IF(AND(E87="done", F87="done"), A87, "")</f>
         <v/>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C88" s="3" t="n">
         <v>1</v>
@@ -2252,14 +2750,23 @@
       <c r="E88" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J88" s="3" t="str">
+      <c r="F88" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G88" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H88" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K88" s="3" t="str">
         <f aca="false">IF(AND(E88="done", F88="done"), A88, "")</f>
         <v/>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C89" s="3" t="n">
         <v>1</v>
@@ -2270,20 +2777,23 @@
       <c r="E89" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F89" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G89" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J89" s="3" t="str">
+      <c r="F89" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G89" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H89" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K89" s="3" t="str">
         <f aca="false">IF(AND(E89="done", F89="done"), A89, "")</f>
         <v/>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C90" s="3" t="n">
         <v>1</v>
@@ -2294,14 +2804,23 @@
       <c r="E90" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J90" s="3" t="str">
+      <c r="F90" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G90" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H90" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K90" s="3" t="str">
         <f aca="false">IF(AND(E90="done", F90="done"), A90, "")</f>
         <v/>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C91" s="3" t="n">
         <v>1</v>
@@ -2318,14 +2837,17 @@
       <c r="G91" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J91" s="3" t="str">
+      <c r="H91" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K91" s="3" t="str">
         <f aca="false">IF(AND(E91="done", F91="done"), A91, "")</f>
         <v/>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C92" s="3" t="n">
         <v>1</v>
@@ -2336,15 +2858,23 @@
       <c r="E92" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F92" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G92" s="3"/>
-      <c r="J92" s="3"/>
+      <c r="F92" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G92" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H92" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K92" s="3" t="str">
+        <f aca="false">IF(AND(E92="done", F92="done"), A92, "")</f>
+        <v/>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C93" s="3" t="n">
         <v>1</v>
@@ -2355,35 +2885,199 @@
       <c r="E93" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J93" s="3" t="str">
+      <c r="F93" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G93" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H93" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K93" s="3" t="str">
         <f aca="false">IF(AND(E93="done", F93="done"), A93, "")</f>
         <v/>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2" t="n">
-        <f aca="false">SUM(C2:C93)</f>
-        <v>85</v>
-      </c>
-      <c r="D94" s="2" t="n">
-        <f aca="false">SUM(D2:D93)</f>
-        <v>85</v>
-      </c>
-      <c r="E94" s="2" t="n">
-        <f aca="false">SUM(E2:E93)</f>
-        <v>85</v>
-      </c>
-      <c r="F94" s="2" t="n">
-        <f aca="false">SUM(F2:F93)</f>
-        <v>52</v>
-      </c>
-      <c r="G94" s="2" t="n">
-        <f aca="false">SUM(G2:G93)</f>
-        <v>47</v>
+      <c r="A94" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C94" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D94" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E94" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F94" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G94" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H94" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K94" s="3" t="str">
+        <f aca="false">IF(AND(E94="done", F94="done"), A94, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C95" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D95" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E95" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F95" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G95" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H95" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K95" s="3" t="str">
+        <f aca="false">IF(AND(E95="done", F95="done"), A95, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C96" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D96" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E96" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F96" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G96" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H96" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K96" s="3" t="str">
+        <f aca="false">IF(AND(E96="done", F96="done"), A96, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="I97" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="K97" s="3"/>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C98" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D98" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E98" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F98" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G98" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H98" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K98" s="3"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C99" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D99" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E99" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F99" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G99" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H99" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K99" s="3" t="str">
+        <f aca="false">IF(AND(E99="done", F99="done"), A99, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2" t="n">
+        <f aca="false">SUM(C2:C99)</f>
+        <v>95</v>
+      </c>
+      <c r="D100" s="2" t="n">
+        <f aca="false">SUM(D2:D99)</f>
+        <v>95</v>
+      </c>
+      <c r="E100" s="2" t="n">
+        <f aca="false">SUM(E2:E99)</f>
+        <v>95</v>
+      </c>
+      <c r="F100" s="2" t="n">
+        <f aca="false">SUM(F2:F99)</f>
+        <v>92</v>
+      </c>
+      <c r="G100" s="2" t="n">
+        <f aca="false">SUM(G2:G99)</f>
+        <v>91</v>
+      </c>
+      <c r="H100" s="2" t="n">
+        <f aca="false">SUM(H2:H99)</f>
+        <v>91</v>
+      </c>
+      <c r="K100" s="1" t="n">
+        <f aca="false">85-52</f>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2412,242 +3106,242 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>108</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>